<commit_message>
Ajuste publicacion 1 Tema 11 sexto
Ajuste publicacion 1 tema 11 sexto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion14/Escaleta_MA_06_14_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion14/Escaleta_MA_06_14_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -489,9 +489,6 @@
   </si>
   <si>
     <t>Determina la moda, la mediana y la media</t>
-  </si>
-  <si>
-    <t>Actividad que propone hallar medidas de tendencia central en situaciones reales</t>
   </si>
   <si>
     <t>Refuerza tu aprendizaje: Los parámetros estadísticos</t>
@@ -915,14 +912,24 @@
       <t>la estadística en Colombia</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Actividad sobre Las medidas de tendencia central </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1242,18 +1249,18 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1264,8 +1271,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1274,94 +1281,94 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1377,7 +1384,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1386,13 +1393,13 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1407,11 +1414,44 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1419,62 +1459,32 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1793,8 +1803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1823,94 +1833,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="38" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="76" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="75" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="F1" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="G1" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="86" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="90" t="s">
+      <c r="I1" s="88" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="92" t="s">
+      <c r="J1" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="78" t="s">
+        <v>211</v>
+      </c>
+      <c r="L1" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="80"/>
+      <c r="O1" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="74" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="82" t="s">
-        <v>212</v>
-      </c>
-      <c r="L1" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="84"/>
-      <c r="O1" s="73" t="s">
-        <v>94</v>
-      </c>
-      <c r="P1" s="73" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q1" s="78" t="s">
+      <c r="Q1" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="77" t="s">
+      <c r="R1" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="75" t="s">
+      <c r="S1" s="91" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="76" t="s">
+      <c r="T1" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="75" t="s">
+      <c r="U1" s="91" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:47" s="38" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A2" s="80"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="81"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="77"/>
       <c r="M2" s="39" t="s">
         <v>89</v>
       </c>
       <c r="N2" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="O2" s="73"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="75"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="91"/>
     </row>
     <row r="3" spans="1:47" ht="16" thickTop="1">
       <c r="A3" s="30" t="s">
@@ -1928,7 +1938,7 @@
       <c r="E3" s="31"/>
       <c r="F3" s="64"/>
       <c r="G3" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H3" s="35">
         <v>1</v>
@@ -1937,7 +1947,7 @@
         <v>23</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K3" s="33" t="s">
         <v>95</v>
@@ -1959,16 +1969,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="S3" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="S3" s="57" t="s">
+      <c r="T3" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="T3" s="59" t="s">
+      <c r="U3" s="57" t="s">
         <v>192</v>
-      </c>
-      <c r="U3" s="57" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:47" s="36" customFormat="1" ht="15">
@@ -1987,7 +1997,7 @@
       </c>
       <c r="F4" s="64"/>
       <c r="G4" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H4" s="35">
         <v>2</v>
@@ -1996,10 +2006,10 @@
         <v>24</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L4" s="32"/>
       <c r="M4" s="34"/>
@@ -2014,16 +2024,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S4" s="60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T4" s="62" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U4" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:47" ht="15">
@@ -2053,7 +2063,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K5" s="33" t="s">
         <v>95</v>
@@ -2075,16 +2085,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S5" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="T5" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="T5" s="62" t="s">
+      <c r="U5" s="60" t="s">
         <v>198</v>
-      </c>
-      <c r="U5" s="60" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:47" s="36" customFormat="1" ht="15">
@@ -2105,7 +2115,7 @@
       </c>
       <c r="F6" s="65"/>
       <c r="G6" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H6" s="41">
         <v>4</v>
@@ -2117,7 +2127,7 @@
         <v>108</v>
       </c>
       <c r="K6" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L6" s="32" t="s">
         <v>76</v>
@@ -2188,7 +2198,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="65"/>
       <c r="G7" s="71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H7" s="41">
         <v>5</v>
@@ -2197,7 +2207,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K7" s="33" t="s">
         <v>95</v>
@@ -2219,16 +2229,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="S7" s="60" t="s">
         <v>194</v>
       </c>
-      <c r="S7" s="60" t="s">
+      <c r="T7" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="U7" s="60" t="s">
         <v>195</v>
-      </c>
-      <c r="T7" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="U7" s="60" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:47" s="36" customFormat="1" ht="15">
@@ -2248,8 +2258,8 @@
         <v>118</v>
       </c>
       <c r="F8" s="65"/>
-      <c r="G8" s="94" t="s">
-        <v>248</v>
+      <c r="G8" s="73" t="s">
+        <v>247</v>
       </c>
       <c r="H8" s="35">
         <v>6</v>
@@ -2280,16 +2290,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S8" s="60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T8" s="62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U8" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:47" ht="15">
@@ -2341,16 +2351,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S9" s="60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T9" s="62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U9" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:47" ht="15">
@@ -2371,7 +2381,7 @@
       </c>
       <c r="F10" s="65"/>
       <c r="G10" s="71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H10" s="41">
         <v>8</v>
@@ -2383,7 +2393,7 @@
         <v>124</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L10" s="32" t="s">
         <v>76</v>
@@ -2440,7 +2450,7 @@
         <v>128</v>
       </c>
       <c r="K11" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L11" s="32" t="s">
         <v>75</v>
@@ -2494,7 +2504,7 @@
         <v>23</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K12" s="33" t="s">
         <v>95</v>
@@ -2516,16 +2526,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="S12" s="60" t="s">
         <v>194</v>
       </c>
-      <c r="S12" s="60" t="s">
+      <c r="T12" s="62" t="s">
+        <v>202</v>
+      </c>
+      <c r="U12" s="60" t="s">
         <v>195</v>
-      </c>
-      <c r="T12" s="62" t="s">
-        <v>203</v>
-      </c>
-      <c r="U12" s="60" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:47" ht="15">
@@ -2558,7 +2568,7 @@
         <v>140</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L13" s="32" t="s">
         <v>76</v>
@@ -2614,10 +2624,10 @@
         <v>24</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L14" s="32" t="s">
         <v>76</v>
@@ -2664,7 +2674,7 @@
       </c>
       <c r="F15" s="65"/>
       <c r="G15" s="71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H15" s="41">
         <v>13</v>
@@ -2676,7 +2686,7 @@
         <v>132</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L15" s="32" t="s">
         <v>76</v>
@@ -2720,7 +2730,7 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="65"/>
-      <c r="G16" s="43" t="s">
+      <c r="G16" s="95" t="s">
         <v>137</v>
       </c>
       <c r="H16" s="41">
@@ -2733,7 +2743,7 @@
         <v>138</v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L16" s="32" t="s">
         <v>75</v>
@@ -2779,7 +2789,7 @@
         <v>148</v>
       </c>
       <c r="F17" s="65"/>
-      <c r="G17" s="43" t="s">
+      <c r="G17" s="95" t="s">
         <v>149</v>
       </c>
       <c r="H17" s="41">
@@ -2789,10 +2799,10 @@
         <v>24</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K17" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L17" s="32" t="s">
         <v>76</v>
@@ -2836,7 +2846,7 @@
         <v>148</v>
       </c>
       <c r="F18" s="65"/>
-      <c r="G18" s="43" t="s">
+      <c r="G18" s="95" t="s">
         <v>150</v>
       </c>
       <c r="H18" s="35">
@@ -2846,10 +2856,10 @@
         <v>24</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L18" s="32" t="s">
         <v>76</v>
@@ -2895,7 +2905,7 @@
         <v>148</v>
       </c>
       <c r="F19" s="65"/>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="95" t="s">
         <v>153</v>
       </c>
       <c r="H19" s="35">
@@ -2905,10 +2915,10 @@
         <v>24</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L19" s="32" t="s">
         <v>76</v>
@@ -2948,12 +2958,12 @@
         <v>100</v>
       </c>
       <c r="D20" s="54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="65"/>
-      <c r="G20" s="43" t="s">
-        <v>159</v>
+      <c r="G20" s="95" t="s">
+        <v>158</v>
       </c>
       <c r="H20" s="41">
         <v>18</v>
@@ -2962,7 +2972,7 @@
         <v>23</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K20" s="33" t="s">
         <v>95</v>
@@ -2975,7 +2985,7 @@
       </c>
       <c r="N20" s="34"/>
       <c r="O20" s="65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P20" s="69" t="s">
         <v>23</v>
@@ -2984,16 +2994,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="S20" s="60" t="s">
         <v>194</v>
       </c>
-      <c r="S20" s="60" t="s">
+      <c r="T20" s="62" t="s">
+        <v>203</v>
+      </c>
+      <c r="U20" s="60" t="s">
         <v>195</v>
-      </c>
-      <c r="T20" s="62" t="s">
-        <v>204</v>
-      </c>
-      <c r="U20" s="60" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15">
@@ -3013,8 +3023,8 @@
         <v>107</v>
       </c>
       <c r="F21" s="65"/>
-      <c r="G21" s="71" t="s">
-        <v>232</v>
+      <c r="G21" s="95" t="s">
+        <v>231</v>
       </c>
       <c r="H21" s="41">
         <v>19</v>
@@ -3023,10 +3033,10 @@
         <v>24</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>156</v>
+        <v>249</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L21" s="32" t="s">
         <v>76</v>
@@ -3034,7 +3044,7 @@
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
       <c r="O21" s="65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P21" s="69" t="s">
         <v>23</v>
@@ -3049,7 +3059,7 @@
         <v>111</v>
       </c>
       <c r="T21" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U21" s="60" t="s">
         <v>113</v>
@@ -3066,14 +3076,14 @@
         <v>100</v>
       </c>
       <c r="D22" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="F22" s="65"/>
       <c r="G22" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H22" s="41">
         <v>20</v>
@@ -3082,10 +3092,10 @@
         <v>24</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L22" s="32" t="s">
         <v>76</v>
@@ -3093,7 +3103,7 @@
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
       <c r="O22" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P22" s="69" t="s">
         <v>23</v>
@@ -3108,7 +3118,7 @@
         <v>111</v>
       </c>
       <c r="T22" s="63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U22" s="60" t="s">
         <v>113</v>
@@ -3125,14 +3135,14 @@
         <v>100</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F23" s="65"/>
       <c r="G23" s="43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H23" s="35">
         <v>21</v>
@@ -3141,10 +3151,10 @@
         <v>23</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L23" s="32" t="s">
         <v>75</v>
@@ -3152,7 +3162,7 @@
       <c r="M23" s="34"/>
       <c r="N23" s="34"/>
       <c r="O23" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P23" s="69" t="s">
         <v>23</v>
@@ -3167,7 +3177,7 @@
         <v>111</v>
       </c>
       <c r="T23" s="63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="U23" s="60" t="s">
         <v>113</v>
@@ -3184,14 +3194,14 @@
         <v>100</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F24" s="65"/>
       <c r="G24" s="43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H24" s="35">
         <v>22</v>
@@ -3200,7 +3210,7 @@
         <v>24</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K24" s="33" t="s">
         <v>95</v>
@@ -3213,7 +3223,7 @@
         <v>92</v>
       </c>
       <c r="O24" s="65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P24" s="69" t="s">
         <v>23</v>
@@ -3222,16 +3232,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S24" s="60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T24" s="62" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="U24" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15">
@@ -3245,14 +3255,14 @@
         <v>100</v>
       </c>
       <c r="D25" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F25" s="65"/>
       <c r="G25" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H25" s="41">
         <v>23</v>
@@ -3261,10 +3271,10 @@
         <v>24</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L25" s="32" t="s">
         <v>76</v>
@@ -3285,7 +3295,7 @@
         <v>111</v>
       </c>
       <c r="T25" s="63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U25" s="60" t="s">
         <v>113</v>
@@ -3302,14 +3312,14 @@
         <v>100</v>
       </c>
       <c r="D26" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F26" s="65"/>
       <c r="G26" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H26" s="41">
         <v>24</v>
@@ -3318,10 +3328,10 @@
         <v>24</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L26" s="32" t="s">
         <v>76</v>
@@ -3329,7 +3339,7 @@
       <c r="M26" s="34"/>
       <c r="N26" s="34"/>
       <c r="O26" s="65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P26" s="69" t="s">
         <v>23</v>
@@ -3344,7 +3354,7 @@
         <v>111</v>
       </c>
       <c r="T26" s="63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U26" s="60" t="s">
         <v>113</v>
@@ -3361,14 +3371,14 @@
         <v>100</v>
       </c>
       <c r="D27" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F27" s="65"/>
       <c r="G27" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H27" s="41">
         <v>25</v>
@@ -3377,10 +3387,10 @@
         <v>24</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K27" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L27" s="32" t="s">
         <v>76</v>
@@ -3388,7 +3398,7 @@
       <c r="M27" s="34"/>
       <c r="N27" s="34"/>
       <c r="O27" s="65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P27" s="69" t="s">
         <v>23</v>
@@ -3403,7 +3413,7 @@
         <v>111</v>
       </c>
       <c r="T27" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U27" s="60" t="s">
         <v>113</v>
@@ -3420,14 +3430,14 @@
         <v>100</v>
       </c>
       <c r="D28" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F28" s="65"/>
       <c r="G28" s="43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H28" s="35">
         <v>26</v>
@@ -3436,10 +3446,10 @@
         <v>24</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L28" s="32" t="s">
         <v>76</v>
@@ -3447,7 +3457,7 @@
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
       <c r="O28" s="65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P28" s="69" t="s">
         <v>24</v>
@@ -3462,7 +3472,7 @@
         <v>111</v>
       </c>
       <c r="T28" s="63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U28" s="60" t="s">
         <v>113</v>
@@ -3479,14 +3489,14 @@
         <v>100</v>
       </c>
       <c r="D29" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>107</v>
       </c>
       <c r="F29" s="65"/>
       <c r="G29" s="72" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H29" s="35">
         <v>27</v>
@@ -3495,10 +3505,10 @@
         <v>24</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K29" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L29" s="32" t="s">
         <v>76</v>
@@ -3506,7 +3516,7 @@
       <c r="M29" s="34"/>
       <c r="N29" s="34"/>
       <c r="O29" s="65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P29" s="69" t="s">
         <v>23</v>
@@ -3521,7 +3531,7 @@
         <v>111</v>
       </c>
       <c r="T29" s="63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U29" s="60" t="s">
         <v>113</v>
@@ -3542,8 +3552,8 @@
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="65"/>
-      <c r="G30" s="94" t="s">
-        <v>249</v>
+      <c r="G30" s="73" t="s">
+        <v>248</v>
       </c>
       <c r="H30" s="41">
         <v>28</v>
@@ -3552,10 +3562,10 @@
         <v>24</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L30" s="32" t="s">
         <v>76</v>
@@ -3563,7 +3573,7 @@
       <c r="M30" s="34"/>
       <c r="N30" s="34"/>
       <c r="O30" s="65" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P30" s="69" t="s">
         <v>23</v>
@@ -3578,7 +3588,7 @@
         <v>111</v>
       </c>
       <c r="T30" s="63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U30" s="60" t="s">
         <v>113</v>
@@ -3600,7 +3610,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="65"/>
       <c r="G31" s="43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H31" s="41">
         <v>29</v>
@@ -3609,10 +3619,10 @@
         <v>24</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L31" s="32" t="s">
         <v>75</v>
@@ -3620,7 +3630,7 @@
       <c r="M31" s="34"/>
       <c r="N31" s="34"/>
       <c r="O31" s="65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P31" s="69" t="s">
         <v>23</v>
@@ -3635,7 +3645,7 @@
         <v>111</v>
       </c>
       <c r="T31" s="63" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U31" s="60" t="s">
         <v>113</v>
@@ -3652,7 +3662,7 @@
         <v>100</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>14</v>
@@ -3664,7 +3674,7 @@
       </c>
       <c r="I32" s="40"/>
       <c r="J32" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K32" s="33"/>
       <c r="L32" s="32"/>
@@ -3691,14 +3701,14 @@
         <v>100</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F33" s="65"/>
       <c r="G33" s="43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H33" s="35">
         <v>31</v>
@@ -3707,7 +3717,7 @@
         <v>24</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K33" s="33" t="s">
         <v>95</v>
@@ -3720,7 +3730,7 @@
         <v>93</v>
       </c>
       <c r="O33" s="65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P33" s="69" t="s">
         <v>23</v>
@@ -3729,16 +3739,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S33" s="60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T33" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U33" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:21" s="36" customFormat="1" ht="15">
@@ -3766,7 +3776,7 @@
         <v>24</v>
       </c>
       <c r="J34" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K34" s="33" t="s">
         <v>95</v>
@@ -3786,16 +3796,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S34" s="60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T34" s="62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U34" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="88" spans="7:7">
@@ -4070,6 +4080,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -4084,12 +4100,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V20 P3">
@@ -4112,7 +4122,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>